<commit_message>
Added Changes to Absences.xlsx
Modified Absences.xlsx
</commit_message>
<xml_diff>
--- a/On-Call-Tracker/src/inputs/Absences.xlsx
+++ b/On-Call-Tracker/src/inputs/Absences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fall 2022\cs2043\Git Repo\OCT-T9\On-Call-Tracker\src\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E0E5C1-E8EB-4A14-930E-145EE2A1A616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE7E42E-DB19-4806-AB23-FBF5FDBC5663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="4215" windowWidth="16200" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week1" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="74">
   <si>
     <t>P2</t>
   </si>
@@ -830,7 +830,7 @@
   <dimension ref="A1:U69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,7 +943,9 @@
         <v>73</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="E3" s="7"/>
       <c r="F3" s="6"/>
       <c r="G3" s="3"/>

</xml_diff>

<commit_message>
Update the Output Excel file.
Added two new columns to Output Excel file.
</commit_message>
<xml_diff>
--- a/On-Call-Tracker/src/inputs/Absences.xlsx
+++ b/On-Call-Tracker/src/inputs/Absences.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fall 2022\cs2043\Git Repo\OCT-T9\On-Call-Tracker\src\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineth/repos/OCT-T9/On-Call-Tracker/src/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE7E42E-DB19-4806-AB23-FBF5FDBC5663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B4081E-0094-9A42-8F55-4FEAF7112A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="4215" windowWidth="16200" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="75000" yWindow="7620" windowWidth="16200" windowHeight="11380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week1" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="74">
   <si>
     <t>P2</t>
   </si>
@@ -829,17 +829,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267BC0D4-2DE4-4A45-B4B4-B0FB4C2E6F0B}">
   <dimension ref="A1:U69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="21" width="4.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="2" max="21" width="4.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="11"/>
       <c r="B1" s="16" t="s">
         <v>4</v>
@@ -872,7 +872,7 @@
       <c r="T1" s="17"/>
       <c r="U1" s="18"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="4" t="s">
         <v>3</v>
@@ -935,7 +935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>9</v>
       </c>
@@ -964,7 +964,7 @@
       <c r="T3" s="3"/>
       <c r="U3" s="7"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>10</v>
       </c>
@@ -991,7 +991,7 @@
       <c r="T4" s="3"/>
       <c r="U4" s="7"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>11</v>
       </c>
@@ -1018,7 +1018,7 @@
       <c r="T5" s="3"/>
       <c r="U5" s="7"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
@@ -1045,7 +1045,7 @@
       <c r="T6" s="3"/>
       <c r="U6" s="7"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>13</v>
       </c>
@@ -1072,7 +1072,7 @@
       <c r="T7" s="3"/>
       <c r="U7" s="7"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>14</v>
       </c>
@@ -1099,7 +1099,7 @@
       <c r="T8" s="3"/>
       <c r="U8" s="7"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>15</v>
       </c>
@@ -1126,7 +1126,7 @@
       <c r="T9" s="3"/>
       <c r="U9" s="7"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>16</v>
       </c>
@@ -1153,7 +1153,7 @@
       <c r="T10" s="3"/>
       <c r="U10" s="7"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>17</v>
       </c>
@@ -1178,7 +1178,7 @@
       <c r="T11" s="3"/>
       <c r="U11" s="7"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>18</v>
       </c>
@@ -1203,7 +1203,7 @@
       <c r="T12" s="3"/>
       <c r="U12" s="7"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>19</v>
       </c>
@@ -1228,7 +1228,7 @@
       <c r="T13" s="3"/>
       <c r="U13" s="7"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>20</v>
       </c>
@@ -1253,7 +1253,7 @@
       <c r="T14" s="3"/>
       <c r="U14" s="7"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -1278,7 +1278,7 @@
       <c r="T15" s="3"/>
       <c r="U15" s="7"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>22</v>
       </c>
@@ -1303,7 +1303,7 @@
       <c r="T16" s="3"/>
       <c r="U16" s="7"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>23</v>
       </c>
@@ -1328,7 +1328,7 @@
       <c r="T17" s="3"/>
       <c r="U17" s="7"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>24</v>
       </c>
@@ -1353,7 +1353,7 @@
       <c r="T18" s="3"/>
       <c r="U18" s="7"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>25</v>
       </c>
@@ -1378,7 +1378,7 @@
       <c r="T19" s="3"/>
       <c r="U19" s="7"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>26</v>
       </c>
@@ -1403,7 +1403,7 @@
       <c r="T20" s="3"/>
       <c r="U20" s="7"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>27</v>
       </c>
@@ -1428,7 +1428,7 @@
       <c r="T21" s="3"/>
       <c r="U21" s="7"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>28</v>
       </c>
@@ -1453,11 +1453,13 @@
       <c r="T22" s="3"/>
       <c r="U22" s="7"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="6" t="s">
+        <v>73</v>
+      </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="7"/>
@@ -1478,7 +1480,7 @@
       <c r="T23" s="3"/>
       <c r="U23" s="7"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
         <v>30</v>
       </c>
@@ -1503,7 +1505,7 @@
       <c r="T24" s="3"/>
       <c r="U24" s="7"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>31</v>
       </c>
@@ -1528,7 +1530,7 @@
       <c r="T25" s="3"/>
       <c r="U25" s="7"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
         <v>32</v>
       </c>
@@ -1553,7 +1555,7 @@
       <c r="T26" s="3"/>
       <c r="U26" s="7"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>33</v>
       </c>
@@ -1578,7 +1580,7 @@
       <c r="T27" s="3"/>
       <c r="U27" s="7"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>34</v>
       </c>
@@ -1603,7 +1605,7 @@
       <c r="T28" s="3"/>
       <c r="U28" s="7"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>35</v>
       </c>
@@ -1628,7 +1630,7 @@
       <c r="T29" s="3"/>
       <c r="U29" s="7"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
         <v>36</v>
       </c>
@@ -1653,7 +1655,7 @@
       <c r="T30" s="3"/>
       <c r="U30" s="7"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>37</v>
       </c>
@@ -1678,7 +1680,7 @@
       <c r="T31" s="3"/>
       <c r="U31" s="7"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>38</v>
       </c>
@@ -1703,7 +1705,7 @@
       <c r="T32" s="3"/>
       <c r="U32" s="7"/>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>39</v>
       </c>
@@ -1728,7 +1730,7 @@
       <c r="T33" s="3"/>
       <c r="U33" s="7"/>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>40</v>
       </c>
@@ -1753,7 +1755,7 @@
       <c r="T34" s="3"/>
       <c r="U34" s="7"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
         <v>41</v>
       </c>
@@ -1778,7 +1780,7 @@
       <c r="T35" s="3"/>
       <c r="U35" s="7"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>42</v>
       </c>
@@ -1803,7 +1805,7 @@
       <c r="T36" s="3"/>
       <c r="U36" s="7"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>43</v>
       </c>
@@ -1828,7 +1830,7 @@
       <c r="T37" s="3"/>
       <c r="U37" s="7"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
         <v>44</v>
       </c>
@@ -1853,7 +1855,7 @@
       <c r="T38" s="3"/>
       <c r="U38" s="7"/>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
         <v>45</v>
       </c>
@@ -1878,7 +1880,7 @@
       <c r="T39" s="3"/>
       <c r="U39" s="7"/>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="13" t="s">
         <v>46</v>
       </c>
@@ -1903,7 +1905,7 @@
       <c r="T40" s="3"/>
       <c r="U40" s="7"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
         <v>47</v>
       </c>
@@ -1928,7 +1930,7 @@
       <c r="T41" s="3"/>
       <c r="U41" s="7"/>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>48</v>
       </c>
@@ -1953,7 +1955,7 @@
       <c r="T42" s="3"/>
       <c r="U42" s="7"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
         <v>49</v>
       </c>
@@ -1978,7 +1980,7 @@
       <c r="T43" s="3"/>
       <c r="U43" s="7"/>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
         <v>50</v>
       </c>
@@ -2003,7 +2005,7 @@
       <c r="T44" s="3"/>
       <c r="U44" s="7"/>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
         <v>51</v>
       </c>
@@ -2028,7 +2030,7 @@
       <c r="T45" s="3"/>
       <c r="U45" s="7"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
         <v>52</v>
       </c>
@@ -2053,7 +2055,7 @@
       <c r="T46" s="3"/>
       <c r="U46" s="7"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
         <v>53</v>
       </c>
@@ -2078,7 +2080,7 @@
       <c r="T47" s="3"/>
       <c r="U47" s="7"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
         <v>54</v>
       </c>
@@ -2103,7 +2105,7 @@
       <c r="T48" s="3"/>
       <c r="U48" s="7"/>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
         <v>55</v>
       </c>
@@ -2128,7 +2130,7 @@
       <c r="T49" s="3"/>
       <c r="U49" s="7"/>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
         <v>56</v>
       </c>
@@ -2153,7 +2155,7 @@
       <c r="T50" s="3"/>
       <c r="U50" s="7"/>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="14" t="s">
         <v>57</v>
       </c>
@@ -2178,7 +2180,7 @@
       <c r="T51" s="3"/>
       <c r="U51" s="7"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
         <v>58</v>
       </c>
@@ -2203,7 +2205,7 @@
       <c r="T52" s="3"/>
       <c r="U52" s="7"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="13" t="s">
         <v>59</v>
       </c>
@@ -2228,7 +2230,7 @@
       <c r="T53" s="3"/>
       <c r="U53" s="7"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
         <v>60</v>
       </c>
@@ -2253,7 +2255,7 @@
       <c r="T54" s="3"/>
       <c r="U54" s="7"/>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
         <v>61</v>
       </c>
@@ -2278,7 +2280,7 @@
       <c r="T55" s="3"/>
       <c r="U55" s="7"/>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
         <v>62</v>
       </c>
@@ -2303,7 +2305,7 @@
       <c r="T56" s="3"/>
       <c r="U56" s="7"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
         <v>63</v>
       </c>
@@ -2328,7 +2330,7 @@
       <c r="T57" s="3"/>
       <c r="U57" s="7"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" s="14" t="s">
         <v>64</v>
       </c>
@@ -2353,7 +2355,7 @@
       <c r="T58" s="3"/>
       <c r="U58" s="7"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
         <v>65</v>
       </c>
@@ -2378,7 +2380,7 @@
       <c r="T59" s="3"/>
       <c r="U59" s="7"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" s="13" t="s">
         <v>66</v>
       </c>
@@ -2403,7 +2405,7 @@
       <c r="T60" s="3"/>
       <c r="U60" s="7"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" s="13" t="s">
         <v>67</v>
       </c>
@@ -2428,7 +2430,7 @@
       <c r="T61" s="3"/>
       <c r="U61" s="7"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" s="14" t="s">
         <v>68</v>
       </c>
@@ -2453,7 +2455,7 @@
       <c r="T62" s="3"/>
       <c r="U62" s="7"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" s="13" t="s">
         <v>69</v>
       </c>
@@ -2478,7 +2480,7 @@
       <c r="T63" s="3"/>
       <c r="U63" s="7"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" s="14" t="s">
         <v>70</v>
       </c>
@@ -2503,7 +2505,7 @@
       <c r="T64" s="3"/>
       <c r="U64" s="7"/>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="14" t="s">
         <v>71</v>
       </c>
@@ -2528,7 +2530,7 @@
       <c r="T65" s="3"/>
       <c r="U65" s="7"/>
     </row>
-    <row r="66" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
         <v>72</v>
       </c>
@@ -2553,13 +2555,13 @@
       <c r="T66" s="9"/>
       <c r="U66" s="10"/>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
     </row>
   </sheetData>
@@ -2583,13 +2585,13 @@
       <selection activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="21" width="4.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="2" max="21" width="4.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="11"/>
       <c r="B1" s="16" t="s">
         <v>4</v>
@@ -2622,7 +2624,7 @@
       <c r="T1" s="17"/>
       <c r="U1" s="18"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="4" t="s">
         <v>3</v>
@@ -2685,7 +2687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>9</v>
       </c>
@@ -2710,7 +2712,7 @@
       <c r="T3" s="3"/>
       <c r="U3" s="7"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>10</v>
       </c>
@@ -2735,7 +2737,7 @@
       <c r="T4" s="3"/>
       <c r="U4" s="7"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>11</v>
       </c>
@@ -2760,7 +2762,7 @@
       <c r="T5" s="3"/>
       <c r="U5" s="7"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
@@ -2785,7 +2787,7 @@
       <c r="T6" s="3"/>
       <c r="U6" s="7"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>13</v>
       </c>
@@ -2810,7 +2812,7 @@
       <c r="T7" s="3"/>
       <c r="U7" s="7"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>14</v>
       </c>
@@ -2835,7 +2837,7 @@
       <c r="T8" s="3"/>
       <c r="U8" s="7"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>15</v>
       </c>
@@ -2860,7 +2862,7 @@
       <c r="T9" s="3"/>
       <c r="U9" s="7"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>16</v>
       </c>
@@ -2885,7 +2887,7 @@
       <c r="T10" s="3"/>
       <c r="U10" s="7"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>17</v>
       </c>
@@ -2910,7 +2912,7 @@
       <c r="T11" s="3"/>
       <c r="U11" s="7"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>18</v>
       </c>
@@ -2935,7 +2937,7 @@
       <c r="T12" s="3"/>
       <c r="U12" s="7"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>19</v>
       </c>
@@ -2960,7 +2962,7 @@
       <c r="T13" s="3"/>
       <c r="U13" s="7"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>20</v>
       </c>
@@ -2985,7 +2987,7 @@
       <c r="T14" s="3"/>
       <c r="U14" s="7"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -3010,7 +3012,7 @@
       <c r="T15" s="3"/>
       <c r="U15" s="7"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>22</v>
       </c>
@@ -3035,7 +3037,7 @@
       <c r="T16" s="3"/>
       <c r="U16" s="7"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>23</v>
       </c>
@@ -3060,7 +3062,7 @@
       <c r="T17" s="3"/>
       <c r="U17" s="7"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>24</v>
       </c>
@@ -3085,7 +3087,7 @@
       <c r="T18" s="3"/>
       <c r="U18" s="7"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>25</v>
       </c>
@@ -3110,7 +3112,7 @@
       <c r="T19" s="3"/>
       <c r="U19" s="7"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>26</v>
       </c>
@@ -3135,7 +3137,7 @@
       <c r="T20" s="3"/>
       <c r="U20" s="7"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>27</v>
       </c>
@@ -3160,7 +3162,7 @@
       <c r="T21" s="3"/>
       <c r="U21" s="7"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>28</v>
       </c>
@@ -3185,7 +3187,7 @@
       <c r="T22" s="3"/>
       <c r="U22" s="7"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>29</v>
       </c>
@@ -3210,7 +3212,7 @@
       <c r="T23" s="3"/>
       <c r="U23" s="7"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
         <v>30</v>
       </c>
@@ -3235,7 +3237,7 @@
       <c r="T24" s="3"/>
       <c r="U24" s="7"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>31</v>
       </c>
@@ -3260,7 +3262,7 @@
       <c r="T25" s="3"/>
       <c r="U25" s="7"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
         <v>32</v>
       </c>
@@ -3285,7 +3287,7 @@
       <c r="T26" s="3"/>
       <c r="U26" s="7"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>33</v>
       </c>
@@ -3310,7 +3312,7 @@
       <c r="T27" s="3"/>
       <c r="U27" s="7"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>34</v>
       </c>
@@ -3335,7 +3337,7 @@
       <c r="T28" s="3"/>
       <c r="U28" s="7"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>35</v>
       </c>
@@ -3360,7 +3362,7 @@
       <c r="T29" s="3"/>
       <c r="U29" s="7"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
         <v>36</v>
       </c>
@@ -3385,7 +3387,7 @@
       <c r="T30" s="3"/>
       <c r="U30" s="7"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>37</v>
       </c>
@@ -3410,7 +3412,7 @@
       <c r="T31" s="3"/>
       <c r="U31" s="7"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>38</v>
       </c>
@@ -3435,7 +3437,7 @@
       <c r="T32" s="3"/>
       <c r="U32" s="7"/>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>39</v>
       </c>
@@ -3460,7 +3462,7 @@
       <c r="T33" s="3"/>
       <c r="U33" s="7"/>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>40</v>
       </c>
@@ -3485,7 +3487,7 @@
       <c r="T34" s="3"/>
       <c r="U34" s="7"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
         <v>41</v>
       </c>
@@ -3510,7 +3512,7 @@
       <c r="T35" s="3"/>
       <c r="U35" s="7"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>42</v>
       </c>
@@ -3535,7 +3537,7 @@
       <c r="T36" s="3"/>
       <c r="U36" s="7"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>43</v>
       </c>
@@ -3560,7 +3562,7 @@
       <c r="T37" s="3"/>
       <c r="U37" s="7"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
         <v>44</v>
       </c>
@@ -3585,7 +3587,7 @@
       <c r="T38" s="3"/>
       <c r="U38" s="7"/>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
         <v>45</v>
       </c>
@@ -3610,7 +3612,7 @@
       <c r="T39" s="3"/>
       <c r="U39" s="7"/>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="13" t="s">
         <v>46</v>
       </c>
@@ -3635,7 +3637,7 @@
       <c r="T40" s="3"/>
       <c r="U40" s="7"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
         <v>47</v>
       </c>
@@ -3660,7 +3662,7 @@
       <c r="T41" s="3"/>
       <c r="U41" s="7"/>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>48</v>
       </c>
@@ -3685,7 +3687,7 @@
       <c r="T42" s="3"/>
       <c r="U42" s="7"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
         <v>49</v>
       </c>
@@ -3710,7 +3712,7 @@
       <c r="T43" s="3"/>
       <c r="U43" s="7"/>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
         <v>50</v>
       </c>
@@ -3735,7 +3737,7 @@
       <c r="T44" s="3"/>
       <c r="U44" s="7"/>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
         <v>51</v>
       </c>
@@ -3760,7 +3762,7 @@
       <c r="T45" s="3"/>
       <c r="U45" s="7"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
         <v>52</v>
       </c>
@@ -3785,7 +3787,7 @@
       <c r="T46" s="3"/>
       <c r="U46" s="7"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
         <v>53</v>
       </c>
@@ -3810,7 +3812,7 @@
       <c r="T47" s="3"/>
       <c r="U47" s="7"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
         <v>54</v>
       </c>
@@ -3835,7 +3837,7 @@
       <c r="T48" s="3"/>
       <c r="U48" s="7"/>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
         <v>55</v>
       </c>
@@ -3860,7 +3862,7 @@
       <c r="T49" s="3"/>
       <c r="U49" s="7"/>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
         <v>56</v>
       </c>
@@ -3885,7 +3887,7 @@
       <c r="T50" s="3"/>
       <c r="U50" s="7"/>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="14" t="s">
         <v>57</v>
       </c>
@@ -3910,7 +3912,7 @@
       <c r="T51" s="3"/>
       <c r="U51" s="7"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
         <v>58</v>
       </c>
@@ -3935,7 +3937,7 @@
       <c r="T52" s="3"/>
       <c r="U52" s="7"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="13" t="s">
         <v>59</v>
       </c>
@@ -3960,7 +3962,7 @@
       <c r="T53" s="3"/>
       <c r="U53" s="7"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
         <v>60</v>
       </c>
@@ -3985,7 +3987,7 @@
       <c r="T54" s="3"/>
       <c r="U54" s="7"/>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
         <v>61</v>
       </c>
@@ -4010,7 +4012,7 @@
       <c r="T55" s="3"/>
       <c r="U55" s="7"/>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
         <v>62</v>
       </c>
@@ -4035,7 +4037,7 @@
       <c r="T56" s="3"/>
       <c r="U56" s="7"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
         <v>63</v>
       </c>
@@ -4060,7 +4062,7 @@
       <c r="T57" s="3"/>
       <c r="U57" s="7"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" s="14" t="s">
         <v>64</v>
       </c>
@@ -4085,7 +4087,7 @@
       <c r="T58" s="3"/>
       <c r="U58" s="7"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
         <v>65</v>
       </c>
@@ -4110,7 +4112,7 @@
       <c r="T59" s="3"/>
       <c r="U59" s="7"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" s="13" t="s">
         <v>66</v>
       </c>
@@ -4135,7 +4137,7 @@
       <c r="T60" s="3"/>
       <c r="U60" s="7"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" s="13" t="s">
         <v>67</v>
       </c>
@@ -4160,7 +4162,7 @@
       <c r="T61" s="3"/>
       <c r="U61" s="7"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" s="14" t="s">
         <v>68</v>
       </c>
@@ -4185,7 +4187,7 @@
       <c r="T62" s="3"/>
       <c r="U62" s="7"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" s="13" t="s">
         <v>69</v>
       </c>
@@ -4210,7 +4212,7 @@
       <c r="T63" s="3"/>
       <c r="U63" s="7"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" s="14" t="s">
         <v>70</v>
       </c>
@@ -4235,7 +4237,7 @@
       <c r="T64" s="3"/>
       <c r="U64" s="7"/>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="14" t="s">
         <v>71</v>
       </c>
@@ -4260,7 +4262,7 @@
       <c r="T65" s="3"/>
       <c r="U65" s="7"/>
     </row>
-    <row r="66" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
         <v>72</v>
       </c>
@@ -4285,13 +4287,13 @@
       <c r="T66" s="9"/>
       <c r="U66" s="10"/>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
     </row>
   </sheetData>
@@ -4315,13 +4317,13 @@
       <selection activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="21" width="4.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="2" max="21" width="4.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="11"/>
       <c r="B1" s="16" t="s">
         <v>4</v>
@@ -4354,7 +4356,7 @@
       <c r="T1" s="17"/>
       <c r="U1" s="18"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="4" t="s">
         <v>3</v>
@@ -4417,7 +4419,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>9</v>
       </c>
@@ -4442,7 +4444,7 @@
       <c r="T3" s="3"/>
       <c r="U3" s="7"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>10</v>
       </c>
@@ -4467,7 +4469,7 @@
       <c r="T4" s="3"/>
       <c r="U4" s="7"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>11</v>
       </c>
@@ -4492,7 +4494,7 @@
       <c r="T5" s="3"/>
       <c r="U5" s="7"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
@@ -4517,7 +4519,7 @@
       <c r="T6" s="3"/>
       <c r="U6" s="7"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>13</v>
       </c>
@@ -4542,7 +4544,7 @@
       <c r="T7" s="3"/>
       <c r="U7" s="7"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>14</v>
       </c>
@@ -4567,7 +4569,7 @@
       <c r="T8" s="3"/>
       <c r="U8" s="7"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>15</v>
       </c>
@@ -4592,7 +4594,7 @@
       <c r="T9" s="3"/>
       <c r="U9" s="7"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>16</v>
       </c>
@@ -4617,7 +4619,7 @@
       <c r="T10" s="3"/>
       <c r="U10" s="7"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>17</v>
       </c>
@@ -4642,7 +4644,7 @@
       <c r="T11" s="3"/>
       <c r="U11" s="7"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>18</v>
       </c>
@@ -4667,7 +4669,7 @@
       <c r="T12" s="3"/>
       <c r="U12" s="7"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>19</v>
       </c>
@@ -4692,7 +4694,7 @@
       <c r="T13" s="3"/>
       <c r="U13" s="7"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>20</v>
       </c>
@@ -4717,7 +4719,7 @@
       <c r="T14" s="3"/>
       <c r="U14" s="7"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -4742,7 +4744,7 @@
       <c r="T15" s="3"/>
       <c r="U15" s="7"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>22</v>
       </c>
@@ -4767,7 +4769,7 @@
       <c r="T16" s="3"/>
       <c r="U16" s="7"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>23</v>
       </c>
@@ -4792,7 +4794,7 @@
       <c r="T17" s="3"/>
       <c r="U17" s="7"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>24</v>
       </c>
@@ -4817,7 +4819,7 @@
       <c r="T18" s="3"/>
       <c r="U18" s="7"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>25</v>
       </c>
@@ -4842,7 +4844,7 @@
       <c r="T19" s="3"/>
       <c r="U19" s="7"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>26</v>
       </c>
@@ -4867,7 +4869,7 @@
       <c r="T20" s="3"/>
       <c r="U20" s="7"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>27</v>
       </c>
@@ -4892,7 +4894,7 @@
       <c r="T21" s="3"/>
       <c r="U21" s="7"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>28</v>
       </c>
@@ -4917,7 +4919,7 @@
       <c r="T22" s="3"/>
       <c r="U22" s="7"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>29</v>
       </c>
@@ -4942,7 +4944,7 @@
       <c r="T23" s="3"/>
       <c r="U23" s="7"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
         <v>30</v>
       </c>
@@ -4967,7 +4969,7 @@
       <c r="T24" s="3"/>
       <c r="U24" s="7"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>31</v>
       </c>
@@ -4992,7 +4994,7 @@
       <c r="T25" s="3"/>
       <c r="U25" s="7"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
         <v>32</v>
       </c>
@@ -5017,7 +5019,7 @@
       <c r="T26" s="3"/>
       <c r="U26" s="7"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>33</v>
       </c>
@@ -5042,7 +5044,7 @@
       <c r="T27" s="3"/>
       <c r="U27" s="7"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>34</v>
       </c>
@@ -5067,7 +5069,7 @@
       <c r="T28" s="3"/>
       <c r="U28" s="7"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>35</v>
       </c>
@@ -5092,7 +5094,7 @@
       <c r="T29" s="3"/>
       <c r="U29" s="7"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
         <v>36</v>
       </c>
@@ -5117,7 +5119,7 @@
       <c r="T30" s="3"/>
       <c r="U30" s="7"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>37</v>
       </c>
@@ -5142,7 +5144,7 @@
       <c r="T31" s="3"/>
       <c r="U31" s="7"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>38</v>
       </c>
@@ -5167,7 +5169,7 @@
       <c r="T32" s="3"/>
       <c r="U32" s="7"/>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>39</v>
       </c>
@@ -5192,7 +5194,7 @@
       <c r="T33" s="3"/>
       <c r="U33" s="7"/>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>40</v>
       </c>
@@ -5217,7 +5219,7 @@
       <c r="T34" s="3"/>
       <c r="U34" s="7"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
         <v>41</v>
       </c>
@@ -5242,7 +5244,7 @@
       <c r="T35" s="3"/>
       <c r="U35" s="7"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>42</v>
       </c>
@@ -5267,7 +5269,7 @@
       <c r="T36" s="3"/>
       <c r="U36" s="7"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>43</v>
       </c>
@@ -5292,7 +5294,7 @@
       <c r="T37" s="3"/>
       <c r="U37" s="7"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
         <v>44</v>
       </c>
@@ -5317,7 +5319,7 @@
       <c r="T38" s="3"/>
       <c r="U38" s="7"/>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
         <v>45</v>
       </c>
@@ -5342,7 +5344,7 @@
       <c r="T39" s="3"/>
       <c r="U39" s="7"/>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="13" t="s">
         <v>46</v>
       </c>
@@ -5367,7 +5369,7 @@
       <c r="T40" s="3"/>
       <c r="U40" s="7"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
         <v>47</v>
       </c>
@@ -5392,7 +5394,7 @@
       <c r="T41" s="3"/>
       <c r="U41" s="7"/>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>48</v>
       </c>
@@ -5417,7 +5419,7 @@
       <c r="T42" s="3"/>
       <c r="U42" s="7"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
         <v>49</v>
       </c>
@@ -5442,7 +5444,7 @@
       <c r="T43" s="3"/>
       <c r="U43" s="7"/>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
         <v>50</v>
       </c>
@@ -5467,7 +5469,7 @@
       <c r="T44" s="3"/>
       <c r="U44" s="7"/>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
         <v>51</v>
       </c>
@@ -5492,7 +5494,7 @@
       <c r="T45" s="3"/>
       <c r="U45" s="7"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
         <v>52</v>
       </c>
@@ -5517,7 +5519,7 @@
       <c r="T46" s="3"/>
       <c r="U46" s="7"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
         <v>53</v>
       </c>
@@ -5542,7 +5544,7 @@
       <c r="T47" s="3"/>
       <c r="U47" s="7"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
         <v>54</v>
       </c>
@@ -5567,7 +5569,7 @@
       <c r="T48" s="3"/>
       <c r="U48" s="7"/>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
         <v>55</v>
       </c>
@@ -5592,7 +5594,7 @@
       <c r="T49" s="3"/>
       <c r="U49" s="7"/>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
         <v>56</v>
       </c>
@@ -5617,7 +5619,7 @@
       <c r="T50" s="3"/>
       <c r="U50" s="7"/>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="14" t="s">
         <v>57</v>
       </c>
@@ -5642,7 +5644,7 @@
       <c r="T51" s="3"/>
       <c r="U51" s="7"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
         <v>58</v>
       </c>
@@ -5667,7 +5669,7 @@
       <c r="T52" s="3"/>
       <c r="U52" s="7"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="13" t="s">
         <v>59</v>
       </c>
@@ -5692,7 +5694,7 @@
       <c r="T53" s="3"/>
       <c r="U53" s="7"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
         <v>60</v>
       </c>
@@ -5717,7 +5719,7 @@
       <c r="T54" s="3"/>
       <c r="U54" s="7"/>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
         <v>61</v>
       </c>
@@ -5742,7 +5744,7 @@
       <c r="T55" s="3"/>
       <c r="U55" s="7"/>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
         <v>62</v>
       </c>
@@ -5767,7 +5769,7 @@
       <c r="T56" s="3"/>
       <c r="U56" s="7"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
         <v>63</v>
       </c>
@@ -5792,7 +5794,7 @@
       <c r="T57" s="3"/>
       <c r="U57" s="7"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" s="14" t="s">
         <v>64</v>
       </c>
@@ -5817,7 +5819,7 @@
       <c r="T58" s="3"/>
       <c r="U58" s="7"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
         <v>65</v>
       </c>
@@ -5842,7 +5844,7 @@
       <c r="T59" s="3"/>
       <c r="U59" s="7"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" s="13" t="s">
         <v>66</v>
       </c>
@@ -5867,7 +5869,7 @@
       <c r="T60" s="3"/>
       <c r="U60" s="7"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" s="13" t="s">
         <v>67</v>
       </c>
@@ -5892,7 +5894,7 @@
       <c r="T61" s="3"/>
       <c r="U61" s="7"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" s="14" t="s">
         <v>68</v>
       </c>
@@ -5917,7 +5919,7 @@
       <c r="T62" s="3"/>
       <c r="U62" s="7"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" s="13" t="s">
         <v>69</v>
       </c>
@@ -5942,7 +5944,7 @@
       <c r="T63" s="3"/>
       <c r="U63" s="7"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" s="14" t="s">
         <v>70</v>
       </c>
@@ -5967,7 +5969,7 @@
       <c r="T64" s="3"/>
       <c r="U64" s="7"/>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="14" t="s">
         <v>71</v>
       </c>
@@ -5992,7 +5994,7 @@
       <c r="T65" s="3"/>
       <c r="U65" s="7"/>
     </row>
-    <row r="66" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
         <v>72</v>
       </c>
@@ -6017,13 +6019,13 @@
       <c r="T66" s="9"/>
       <c r="U66" s="10"/>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
     </row>
   </sheetData>
@@ -6047,13 +6049,13 @@
       <selection activeCell="M70" sqref="M70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="21" width="4.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="2" max="21" width="4.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="11"/>
       <c r="B1" s="16" t="s">
         <v>4</v>
@@ -6086,7 +6088,7 @@
       <c r="T1" s="17"/>
       <c r="U1" s="18"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="4" t="s">
         <v>3</v>
@@ -6149,7 +6151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>9</v>
       </c>
@@ -6174,7 +6176,7 @@
       <c r="T3" s="3"/>
       <c r="U3" s="7"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>10</v>
       </c>
@@ -6199,7 +6201,7 @@
       <c r="T4" s="3"/>
       <c r="U4" s="7"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>11</v>
       </c>
@@ -6224,7 +6226,7 @@
       <c r="T5" s="3"/>
       <c r="U5" s="7"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
@@ -6249,7 +6251,7 @@
       <c r="T6" s="3"/>
       <c r="U6" s="7"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>13</v>
       </c>
@@ -6274,7 +6276,7 @@
       <c r="T7" s="3"/>
       <c r="U7" s="7"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>14</v>
       </c>
@@ -6299,7 +6301,7 @@
       <c r="T8" s="3"/>
       <c r="U8" s="7"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>15</v>
       </c>
@@ -6324,7 +6326,7 @@
       <c r="T9" s="3"/>
       <c r="U9" s="7"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>16</v>
       </c>
@@ -6349,7 +6351,7 @@
       <c r="T10" s="3"/>
       <c r="U10" s="7"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>17</v>
       </c>
@@ -6374,7 +6376,7 @@
       <c r="T11" s="3"/>
       <c r="U11" s="7"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>18</v>
       </c>
@@ -6399,7 +6401,7 @@
       <c r="T12" s="3"/>
       <c r="U12" s="7"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>19</v>
       </c>
@@ -6424,7 +6426,7 @@
       <c r="T13" s="3"/>
       <c r="U13" s="7"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>20</v>
       </c>
@@ -6449,7 +6451,7 @@
       <c r="T14" s="3"/>
       <c r="U14" s="7"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>21</v>
       </c>
@@ -6474,7 +6476,7 @@
       <c r="T15" s="3"/>
       <c r="U15" s="7"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>22</v>
       </c>
@@ -6499,7 +6501,7 @@
       <c r="T16" s="3"/>
       <c r="U16" s="7"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>23</v>
       </c>
@@ -6524,7 +6526,7 @@
       <c r="T17" s="3"/>
       <c r="U17" s="7"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>24</v>
       </c>
@@ -6549,7 +6551,7 @@
       <c r="T18" s="3"/>
       <c r="U18" s="7"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>25</v>
       </c>
@@ -6574,7 +6576,7 @@
       <c r="T19" s="3"/>
       <c r="U19" s="7"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>26</v>
       </c>
@@ -6599,7 +6601,7 @@
       <c r="T20" s="3"/>
       <c r="U20" s="7"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>27</v>
       </c>
@@ -6624,7 +6626,7 @@
       <c r="T21" s="3"/>
       <c r="U21" s="7"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>28</v>
       </c>
@@ -6649,7 +6651,7 @@
       <c r="T22" s="3"/>
       <c r="U22" s="7"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>29</v>
       </c>
@@ -6674,7 +6676,7 @@
       <c r="T23" s="3"/>
       <c r="U23" s="7"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
         <v>30</v>
       </c>
@@ -6699,7 +6701,7 @@
       <c r="T24" s="3"/>
       <c r="U24" s="7"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>31</v>
       </c>
@@ -6724,7 +6726,7 @@
       <c r="T25" s="3"/>
       <c r="U25" s="7"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
         <v>32</v>
       </c>
@@ -6749,7 +6751,7 @@
       <c r="T26" s="3"/>
       <c r="U26" s="7"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>33</v>
       </c>
@@ -6774,7 +6776,7 @@
       <c r="T27" s="3"/>
       <c r="U27" s="7"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>34</v>
       </c>
@@ -6799,7 +6801,7 @@
       <c r="T28" s="3"/>
       <c r="U28" s="7"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>35</v>
       </c>
@@ -6824,7 +6826,7 @@
       <c r="T29" s="3"/>
       <c r="U29" s="7"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
         <v>36</v>
       </c>
@@ -6849,7 +6851,7 @@
       <c r="T30" s="3"/>
       <c r="U30" s="7"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>37</v>
       </c>
@@ -6874,7 +6876,7 @@
       <c r="T31" s="3"/>
       <c r="U31" s="7"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>38</v>
       </c>
@@ -6899,7 +6901,7 @@
       <c r="T32" s="3"/>
       <c r="U32" s="7"/>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>39</v>
       </c>
@@ -6924,7 +6926,7 @@
       <c r="T33" s="3"/>
       <c r="U33" s="7"/>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>40</v>
       </c>
@@ -6949,7 +6951,7 @@
       <c r="T34" s="3"/>
       <c r="U34" s="7"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
         <v>41</v>
       </c>
@@ -6974,7 +6976,7 @@
       <c r="T35" s="3"/>
       <c r="U35" s="7"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>42</v>
       </c>
@@ -6999,7 +7001,7 @@
       <c r="T36" s="3"/>
       <c r="U36" s="7"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>43</v>
       </c>
@@ -7024,7 +7026,7 @@
       <c r="T37" s="3"/>
       <c r="U37" s="7"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
         <v>44</v>
       </c>
@@ -7049,7 +7051,7 @@
       <c r="T38" s="3"/>
       <c r="U38" s="7"/>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
         <v>45</v>
       </c>
@@ -7074,7 +7076,7 @@
       <c r="T39" s="3"/>
       <c r="U39" s="7"/>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="13" t="s">
         <v>46</v>
       </c>
@@ -7099,7 +7101,7 @@
       <c r="T40" s="3"/>
       <c r="U40" s="7"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
         <v>47</v>
       </c>
@@ -7124,7 +7126,7 @@
       <c r="T41" s="3"/>
       <c r="U41" s="7"/>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>48</v>
       </c>
@@ -7149,7 +7151,7 @@
       <c r="T42" s="3"/>
       <c r="U42" s="7"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
         <v>49</v>
       </c>
@@ -7174,7 +7176,7 @@
       <c r="T43" s="3"/>
       <c r="U43" s="7"/>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
         <v>50</v>
       </c>
@@ -7199,7 +7201,7 @@
       <c r="T44" s="3"/>
       <c r="U44" s="7"/>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
         <v>51</v>
       </c>
@@ -7224,7 +7226,7 @@
       <c r="T45" s="3"/>
       <c r="U45" s="7"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
         <v>52</v>
       </c>
@@ -7249,7 +7251,7 @@
       <c r="T46" s="3"/>
       <c r="U46" s="7"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
         <v>53</v>
       </c>
@@ -7274,7 +7276,7 @@
       <c r="T47" s="3"/>
       <c r="U47" s="7"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
         <v>54</v>
       </c>
@@ -7299,7 +7301,7 @@
       <c r="T48" s="3"/>
       <c r="U48" s="7"/>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
         <v>55</v>
       </c>
@@ -7324,7 +7326,7 @@
       <c r="T49" s="3"/>
       <c r="U49" s="7"/>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
         <v>56</v>
       </c>
@@ -7349,7 +7351,7 @@
       <c r="T50" s="3"/>
       <c r="U50" s="7"/>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="14" t="s">
         <v>57</v>
       </c>
@@ -7374,7 +7376,7 @@
       <c r="T51" s="3"/>
       <c r="U51" s="7"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
         <v>58</v>
       </c>
@@ -7399,7 +7401,7 @@
       <c r="T52" s="3"/>
       <c r="U52" s="7"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="13" t="s">
         <v>59</v>
       </c>
@@ -7424,7 +7426,7 @@
       <c r="T53" s="3"/>
       <c r="U53" s="7"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
         <v>60</v>
       </c>
@@ -7449,7 +7451,7 @@
       <c r="T54" s="3"/>
       <c r="U54" s="7"/>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
         <v>61</v>
       </c>
@@ -7474,7 +7476,7 @@
       <c r="T55" s="3"/>
       <c r="U55" s="7"/>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
         <v>62</v>
       </c>
@@ -7499,7 +7501,7 @@
       <c r="T56" s="3"/>
       <c r="U56" s="7"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
         <v>63</v>
       </c>
@@ -7524,7 +7526,7 @@
       <c r="T57" s="3"/>
       <c r="U57" s="7"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" s="14" t="s">
         <v>64</v>
       </c>
@@ -7549,7 +7551,7 @@
       <c r="T58" s="3"/>
       <c r="U58" s="7"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
         <v>65</v>
       </c>
@@ -7574,7 +7576,7 @@
       <c r="T59" s="3"/>
       <c r="U59" s="7"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" s="13" t="s">
         <v>66</v>
       </c>
@@ -7599,7 +7601,7 @@
       <c r="T60" s="3"/>
       <c r="U60" s="7"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" s="13" t="s">
         <v>67</v>
       </c>
@@ -7624,7 +7626,7 @@
       <c r="T61" s="3"/>
       <c r="U61" s="7"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" s="14" t="s">
         <v>68</v>
       </c>
@@ -7649,7 +7651,7 @@
       <c r="T62" s="3"/>
       <c r="U62" s="7"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" s="13" t="s">
         <v>69</v>
       </c>
@@ -7674,7 +7676,7 @@
       <c r="T63" s="3"/>
       <c r="U63" s="7"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" s="14" t="s">
         <v>70</v>
       </c>
@@ -7699,7 +7701,7 @@
       <c r="T64" s="3"/>
       <c r="U64" s="7"/>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="14" t="s">
         <v>71</v>
       </c>
@@ -7724,7 +7726,7 @@
       <c r="T65" s="3"/>
       <c r="U65" s="7"/>
     </row>
-    <row r="66" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
         <v>72</v>
       </c>
@@ -7749,13 +7751,13 @@
       <c r="T66" s="9"/>
       <c r="U66" s="10"/>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Merge branch 'develop' of https://github.com/myUNB-CSCourses/OCT-T9 into develop"
This reverts commit 252507cc54e9ef04c52998aee6821339c4699cb5, reversing
changes made to 452148316bd435edfe0827db86ef11e08d63597b.
</commit_message>
<xml_diff>
--- a/On-Call-Tracker/src/inputs/Absences.xlsx
+++ b/On-Call-Tracker/src/inputs/Absences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineth/repos/OCT-T9/On-Call-Tracker/src/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1E3880-35A1-F846-AB1A-15BD98D7375D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B4081E-0094-9A42-8F55-4FEAF7112A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="1520" windowWidth="16200" windowHeight="11380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="75000" yWindow="7620" windowWidth="16200" windowHeight="11380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week1" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="74">
   <si>
     <t>P2</t>
   </si>
@@ -830,7 +830,7 @@
   <dimension ref="A1:U69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1130,7 +1130,9 @@
       <c r="A10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>73</v>
+      </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="7"/>
@@ -1458,13 +1460,9 @@
       <c r="B23" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="7" t="s">
-        <v>73</v>
-      </c>
+      <c r="E23" s="7"/>
       <c r="F23" s="6"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -1561,15 +1559,9 @@
       <c r="A27" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
       <c r="E27" s="7"/>
       <c r="F27" s="6"/>
       <c r="G27" s="3"/>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'develop' of https://github.com/myUNB-CSCourses/OCT-T9 into develop""
This reverts commit e51734176237408012b73d6968e7d596d30fc933.
</commit_message>
<xml_diff>
--- a/On-Call-Tracker/src/inputs/Absences.xlsx
+++ b/On-Call-Tracker/src/inputs/Absences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineth/repos/OCT-T9/On-Call-Tracker/src/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B4081E-0094-9A42-8F55-4FEAF7112A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1E3880-35A1-F846-AB1A-15BD98D7375D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75000" yWindow="7620" windowWidth="16200" windowHeight="11380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1660" yWindow="1520" windowWidth="16200" windowHeight="11380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week1" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="74">
   <si>
     <t>P2</t>
   </si>
@@ -830,7 +830,7 @@
   <dimension ref="A1:U69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1130,9 +1130,7 @@
       <c r="A10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>73</v>
-      </c>
+      <c r="B10" s="6"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="7"/>
@@ -1460,9 +1458,13 @@
       <c r="B23" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="D23" s="3"/>
-      <c r="E23" s="7"/>
+      <c r="E23" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="F23" s="6"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -1559,9 +1561,15 @@
       <c r="A27" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="B27" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="E27" s="7"/>
       <c r="F27" s="6"/>
       <c r="G27" s="3"/>

</xml_diff>